<commit_message>
fvsOLdev (bugfix): the table description for the FVS_Carbon table was, for reasons unknown, set to the description for the FVS_ATRTList* tables.
</commit_message>
<xml_diff>
--- a/fvsOLdev/inst/extdata/databaseDescription.xlsx
+++ b/fvsOLdev/inst/extdata/databaseDescription.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitFVS\ForestVegetationSimulator-Interface\fvsOLdev\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A2326D-9942-441E-BFD5-39EC5BF2A361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4534352-A948-478C-84BB-5DACA0C3AA2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColorKey" sheetId="1" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10030" uniqueCount="2885">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10030" uniqueCount="2886">
   <si>
     <t>Tab Color</t>
   </si>
@@ -8803,6 +8803,9 @@
   </si>
   <si>
     <t>https://www.fs.usda.gov/fmsc/ftp/fvs/docs/gtr/EconUserGuide.pdf</t>
+  </si>
+  <si>
+    <t>is generated by the Fire and Fuels Extension. The table contains above and below ground carbon loads for live, dead, snags, down wood, shrubs, and carbon released by fire. There is one row for each stand and cycle year.</t>
   </si>
 </sst>
 </file>
@@ -15884,8 +15887,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ101"/>
   <sheetViews>
-    <sheetView topLeftCell="B36" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="B24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="77.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16116,7 +16119,7 @@
         <v>72</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -16132,7 +16135,7 @@
         <v>75</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>73</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -16140,7 +16143,7 @@
         <v>76</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>73</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -21868,7 +21871,7 @@
   </sheetPr>
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B96" sqref="B96:B101"/>
     </sheetView>
   </sheetViews>

</xml_diff>